<commit_message>
added in sample of API documentation for user
</commit_message>
<xml_diff>
--- a/API_table.xlsx
+++ b/API_table.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F7EFEA-51E8-4720-AA8A-EA00A565082B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F477272-C984-411B-A0BB-337A6CA2F353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8340" yWindow="3180" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API LIST" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>USER APIs</t>
   </si>
@@ -44,6 +50,72 @@
   </si>
   <si>
     <t>Special Notes</t>
+  </si>
+  <si>
+    <t>https://courier50003.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>/user/test</t>
+  </si>
+  <si>
+    <t>/user/signup</t>
+  </si>
+  <si>
+    <t>/portal</t>
+  </si>
+  <si>
+    <t>/portal/test</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String Message 'This is the REQUESTS Test controller!' </t>
+  </si>
+  <si>
+    <t>String Message 'This is the USER_MANAGEMENT Test controller!'</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+  </si>
+  <si>
+    <t>USER_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>USER_MANAGEMENT
+USER_SESSION</t>
+  </si>
+  <si>
+    <t>1) success: Bool
+2) message: String
+3) token: String 
+4) authority: String</t>
+  </si>
+  <si>
+    <t>1) name: String
+2) password: String
+3) contact_num: Long
+4) type: String</t>
+  </si>
+  <si>
+    <t>1) email: String
+2) password: String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) success: Bool
+2) error: Bool
+3) message: String </t>
+  </si>
+  <si>
+    <t>/user/logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) token: String </t>
+  </si>
+  <si>
+    <t>1) success: Bool
+2) message: String
+3) id: String</t>
   </si>
 </sst>
 </file>
@@ -79,8 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,18 +436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -380,49 +455,174 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use case diagram added
</commit_message>
<xml_diff>
--- a/API_table.xlsx
+++ b/API_table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F477272-C984-411B-A0BB-337A6CA2F353}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56DC995-8971-4A2E-AF49-90E1C0CD7941}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8340" yWindow="3180" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API LIST" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
-  <si>
-    <t>USER APIs</t>
-  </si>
-  <si>
-    <t>ADMIN API</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>Server URL</t>
   </si>
@@ -61,19 +55,10 @@
     <t>/user/signup</t>
   </si>
   <si>
-    <t>/portal</t>
-  </si>
-  <si>
     <t>/portal/test</t>
   </si>
   <si>
     <t>NIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String Message 'This is the REQUESTS Test controller!' </t>
-  </si>
-  <si>
-    <t>String Message 'This is the USER_MANAGEMENT Test controller!'</t>
   </si>
   <si>
     <t>/user/login</t>
@@ -116,13 +101,150 @@
     <t>1) success: Bool
 2) message: String
 3) id: String</t>
+  </si>
+  <si>
+    <t>1) Message: 'This is the USER_MANAGEMENT Test controller!'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Message 'This is the REQUESTS Test controller!' </t>
+  </si>
+  <si>
+    <t>/portal/usersubmit</t>
+  </si>
+  <si>
+    <t>/portal/usersubmitacc</t>
+  </si>
+  <si>
+    <t>/portal/adminhandle</t>
+  </si>
+  <si>
+    <t>/portal/admincomplete</t>
+  </si>
+  <si>
+    <t>/portal/adminview</t>
+  </si>
+  <si>
+    <t>/portal/view</t>
+  </si>
+  <si>
+    <t>/portal/chats</t>
+  </si>
+  <si>
+    <t>/portal/viewdate</t>
+  </si>
+  <si>
+    <t>/portal/viewstatus</t>
+  </si>
+  <si>
+    <t>/portal/viewcategory</t>
+  </si>
+  <si>
+    <t>/portal/viewpriority</t>
+  </si>
+  <si>
+    <t>/portal/viewreq</t>
+  </si>
+  <si>
+    <t>USER MANAGEMENT APIs</t>
+  </si>
+  <si>
+    <t>REQUEST APIs</t>
+  </si>
+  <si>
+    <t>1) name: String
+2) message: String
+3) contact_num: Long
+4) img: PNG/JPG
+5) category: String
+6) email: String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) name: String
+2) message: String
+3) contact_num: Long
+4) img: PNG/JPG
+5) category: String
+6) email: String
+6) sentiment: Int
+7) tags: Array of Strings </t>
+  </si>
+  <si>
+    <t>1) User id: String
+2) Message: String
+3) imageURL: String
+4) category: String</t>
+  </si>
+  <si>
+    <t>1) username: String
+2) message: String
+3) contact_num: Long
+4) img: PNG/JPG
+5) category: String
+6) email: String
+6) sentiment: Int
+7) tags: Array of Strings 
+8) name: String</t>
+  </si>
+  <si>
+    <t>REQUESTS</t>
+  </si>
+  <si>
+    <t>Get user credentials from USERMANAGEMENT collection</t>
+  </si>
+  <si>
+    <t>1) admin_id: String
+2) request_id: String 
+3) conversation: String</t>
+  </si>
+  <si>
+    <t>1) Update chat array
+2) success: Boolean 
+3) message: String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) user_id: String </t>
+  </si>
+  <si>
+    <t>1) List of requests (Which are arrays) sorted by date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) user_id: String 
+2) request_id: String </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) View a specific request </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) admin_id: String
+2) request_id: String </t>
+  </si>
+  <si>
+    <t>1) admin_id: String</t>
+  </si>
+  <si>
+    <t>1) View specific requests that are handled by the admin. A list of arrays (which are arrays) sorted by date</t>
+  </si>
+  <si>
+    <t>1) Views all requests in the portal (unsorted)</t>
+  </si>
+  <si>
+    <t>1) success: Boolean
+2) message: String
+3) adminHandle: String (Username of admin)
+Change status of request to complete</t>
+  </si>
+  <si>
+    <t>1) success: Boolean
+2) message: String
+3) adminHandle: String (Username of admin)
+Change status of request to addressing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,16 +252,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -147,15 +289,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,196 +632,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B12:B13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E13:E24"/>
+    <mergeCell ref="D13:D24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>